<commit_message>
modified front end pane
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="mars" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Category</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>3432.0</t>
+  </si>
+  <si>
+    <t>genser</t>
+  </si>
+  <si>
+    <t>1000.0</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -201,6 +207,23 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
finished the gui frontend on all windows. Not connected to backend
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -68,10 +69,28 @@
     <t>3432.0</t>
   </si>
   <si>
+    <t>atb</t>
+  </si>
+  <si>
+    <t>1000.0</t>
+  </si>
+  <si>
+    <t>Savings</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>playstation</t>
+  </si>
+  <si>
+    <t>2023-04-12</t>
+  </si>
+  <si>
+    <t>2000.0</t>
+  </si>
+  <si>
     <t>genser</t>
-  </si>
-  <si>
-    <t>1000.0</t>
   </si>
 </sst>
 </file>
@@ -116,7 +135,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -209,7 +228,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -221,7 +240,71 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deleted dead classes and removed redundant code
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Category</t>
   </si>
@@ -91,6 +91,27 @@
   </si>
   <si>
     <t>genser</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>douchebag</t>
+  </si>
+  <si>
+    <t>2023-03-22</t>
+  </si>
+  <si>
+    <t>4000.0</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>macbook</t>
+  </si>
+  <si>
+    <t>7000.0</t>
   </si>
 </sst>
 </file>
@@ -135,7 +156,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -258,6 +279,40 @@
       </c>
       <c r="E7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed ForgotPassword class so that you can change your password
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Category</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>7000.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monthly total: </t>
   </si>
 </sst>
 </file>
@@ -156,7 +159,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -315,6 +318,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="n">
+        <v>18360.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -322,7 +333,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -362,6 +373,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2000.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
made all back buttons, but you can only go back one time on each
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Category</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>7000.0</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>3000.0</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -159,7 +165,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -320,10 +326,44 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" t="n">
-        <v>18360.0</v>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="n">
+        <v>22360.0</v>
       </c>
     </row>
   </sheetData>
@@ -375,7 +415,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B3" t="n">
         <v>2000.0</v>

</xml_diff>

<commit_message>
updating progress, dont merge
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="March" r:id="rId3" sheetId="1"/>
-    <sheet name="April" r:id="rId4" sheetId="2"/>
+    <sheet name="mars" r:id="rId3" sheetId="1"/>
+    <sheet name="april" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>

<commit_message>
changed the look of transfer and added a button for adding account
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,14 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="46">
   <si>
     <t>Category</t>
   </si>
@@ -118,6 +118,36 @@
   </si>
   <si>
     <t>3000.0</t>
+  </si>
+  <si>
+    <t>pizza</t>
+  </si>
+  <si>
+    <t>2023-03-27</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>asfd</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>elias</t>
+  </si>
+  <si>
+    <t>banan</t>
+  </si>
+  <si>
+    <t>asf</t>
+  </si>
+  <si>
+    <t>234.0</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -165,7 +195,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -360,10 +390,214 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="B12" t="n">
-        <v>22360.0</v>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="n">
+        <v>30894.0</v>
       </c>
     </row>
   </sheetData>
@@ -415,7 +649,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B3" t="n">
         <v>2000.0</v>

</xml_diff>

<commit_message>
fixed possible pipeline error
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Category</t>
   </si>
@@ -38,9 +38,6 @@
     <t>2023-03-29</t>
   </si>
   <si>
-    <t>450.0</t>
-  </si>
-  <si>
     <t>ABCDE</t>
   </si>
   <si>
@@ -48,9 +45,6 @@
   </si>
   <si>
     <t>smwms</t>
-  </si>
-  <si>
-    <t>500.0</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -131,33 +125,33 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2" t="n">
+        <v>450.0</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
+      <c r="D3" t="n">
+        <v>500.0</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="n">
         <v>950.0</v>

</xml_diff>

<commit_message>
fixed issue where if you log in and then log out and go onto another user, it uses the old users info for some areas
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -7,12 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
   <si>
     <t>Category</t>
   </si>
@@ -45,6 +46,48 @@
   </si>
   <si>
     <t>smwms</t>
+  </si>
+  <si>
+    <t>htfg</t>
+  </si>
+  <si>
+    <t>2023-04-19</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>hyfg</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>tfg</t>
+  </si>
+  <si>
+    <t>hjgy</t>
+  </si>
+  <si>
+    <t>Clothing</t>
+  </si>
+  <si>
+    <t>fesd</t>
+  </si>
+  <si>
+    <t>grd</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -151,10 +194,235 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B4" t="n">
         <v>950.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="n">
+        <v>555.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="n">
+        <v>554.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>444.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="n">
+        <v>554.0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="n">
+        <v>999.0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="n">
+        <v>9999.0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="n">
+        <v>23332.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bugs, added error handling in when editing tables
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,14 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="March" r:id="rId3" sheetId="1"/>
-    <sheet name="April" r:id="rId4" sheetId="2"/>
+    <sheet name="mars" r:id="rId3" sheetId="1"/>
+    <sheet name="april" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
   <si>
     <t>Category</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>test2</t>
+  </si>
+  <si>
+    <t>gtdf</t>
   </si>
   <si>
     <t xml:space="preserve">Monthly total: </t>
@@ -194,7 +197,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" t="n">
         <v>950.0</v>
@@ -414,12 +417,12 @@
         <v>9999.0</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B13" t="n">
         <v>23332.0</v>

</xml_diff>

<commit_message>
when you add a value for an existing category and month in Budget, it is now replaced in the budget csv file
</commit_message>
<xml_diff>
--- a/src/main/resources/userfiles/eliastt/eliastt.xlsx
+++ b/src/main/resources/userfiles/eliastt/eliastt.xlsx
@@ -6,8 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="mars" r:id="rId3" sheetId="1"/>
-    <sheet name="april" r:id="rId4" sheetId="2"/>
+    <sheet name="March" r:id="rId3" sheetId="1"/>
+    <sheet name="April" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>

</xml_diff>